<commit_message>
Boolean type check fix.
</commit_message>
<xml_diff>
--- a/tests/datasets/test1_zip.xlsx
+++ b/tests/datasets/test1_zip.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10414"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA58B615-4081-5C4F-9159-BB38ABB6CF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10804BB4-BDA5-6643-A8EE-907E44A68055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10320" yWindow="680" windowWidth="33600" windowHeight="20280" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7720" yWindow="500" windowWidth="33600" windowHeight="20280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schema Description" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="71">
   <si>
     <t>This is an Excel workbook for data entry.</t>
   </si>
@@ -236,7 +236,13 @@
     <t>Striker</t>
   </si>
   <si>
-    <t>f</t>
+    <t>T</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>adadfdfadf</t>
   </si>
 </sst>
 </file>
@@ -697,7 +703,7 @@
   <dimension ref="A2:N45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1146,10 +1152,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1219,6 +1225,11 @@
       </c>
       <c r="J2" s="8">
         <v>45139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1236,8 +1247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1271,19 +1282,15 @@
         <v>52</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="J1" s="7" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <f>IF(ISBLANK('Data Entry'!$A$2), "", 'Data Entry'!$A$2)</f>
-        <v>37</v>
-      </c>
-      <c r="B2" t="b">
-        <v>0</v>
+      <c r="B2" t="s">
+        <v>68</v>
       </c>
       <c r="C2" t="s">
         <v>61</v>
@@ -1318,12 +1325,8 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <f>IF(ISBLANK('Data Entry'!$A$2), "", 'Data Entry'!$A$2)</f>
-        <v>37</v>
-      </c>
-      <c r="B3" t="s">
-        <v>68</v>
+      <c r="B3">
+        <v>2</v>
       </c>
       <c r="C3" t="s">
         <v>61</v>

</xml_diff>